<commit_message>
generates lists of all features
</commit_message>
<xml_diff>
--- a/data/numbeo_col.xlsx
+++ b/data/numbeo_col.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pallavitangirala/Documents/projects/budget-recommender/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{262243E5-E0DB-8B44-9CE7-7364E308FE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F891AE-ED00-5243-8E95-643E1FA28722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="16820" xr2:uid="{A6F58AA9-D937-A947-BCA9-2D39C5F09156}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t>Rent Index</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Tulsa, OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F62098E-CAD1-AC4E-84E3-E6F29159F746}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,1762 +725,3321 @@
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>99.7</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4">
-        <v>92.5</v>
+        <v>100</v>
       </c>
       <c r="E3" s="4">
-        <v>96.2</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4">
-        <v>99.6</v>
+        <v>100</v>
       </c>
       <c r="G3" s="4">
-        <v>98.5</v>
+        <v>100</v>
       </c>
       <c r="H3" s="4">
-        <v>106.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>111.3</v>
+        <v>100</v>
       </c>
       <c r="D4" s="4">
-        <v>88.8</v>
+        <v>100</v>
       </c>
       <c r="E4" s="4">
-        <v>100.6</v>
+        <v>100</v>
       </c>
       <c r="F4" s="4">
-        <v>117.3</v>
+        <v>100</v>
       </c>
       <c r="G4" s="4">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="H4" s="4">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D5" s="4">
-        <v>77.099999999999994</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4">
-        <v>80.2</v>
+        <v>100</v>
       </c>
       <c r="F5" s="4">
-        <v>76.7</v>
+        <v>100</v>
       </c>
       <c r="G5" s="4">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="H5" s="4">
-        <v>117.3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>85.1</v>
+        <v>100</v>
       </c>
       <c r="D6" s="4">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="E6" s="4">
-        <v>80.8</v>
+        <v>100</v>
       </c>
       <c r="F6" s="4">
-        <v>83.3</v>
+        <v>100</v>
       </c>
       <c r="G6" s="4">
-        <v>87.5</v>
+        <v>100</v>
       </c>
       <c r="H6" s="4">
-        <v>110.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D7" s="4">
-        <v>74.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="E7" s="4">
-        <v>84.7</v>
+        <v>100</v>
       </c>
       <c r="F7" s="4">
-        <v>96.7</v>
+        <v>100</v>
       </c>
       <c r="G7" s="4">
-        <v>85.5</v>
+        <v>100</v>
       </c>
       <c r="H7" s="4">
-        <v>96.3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
-        <v>79.2</v>
+        <v>100</v>
       </c>
       <c r="D8" s="4">
-        <v>73.8</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4">
-        <v>76.599999999999994</v>
+        <v>100</v>
       </c>
       <c r="F8" s="4">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="G8" s="4">
-        <v>88.7</v>
+        <v>100</v>
       </c>
       <c r="H8" s="4">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" s="4">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D9" s="4">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="E9" s="4">
-        <v>79.3</v>
+        <v>100</v>
       </c>
       <c r="F9" s="4">
-        <v>80.099999999999994</v>
+        <v>100</v>
       </c>
       <c r="G9" s="4">
-        <v>83.8</v>
+        <v>100</v>
       </c>
       <c r="H9" s="4">
-        <v>143.6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
-        <v>81.2</v>
+        <v>100</v>
       </c>
       <c r="D10" s="4">
-        <v>71.2</v>
+        <v>100</v>
       </c>
       <c r="E10" s="4">
-        <v>76.400000000000006</v>
+        <v>100</v>
       </c>
       <c r="F10" s="4">
-        <v>79.5</v>
+        <v>100</v>
       </c>
       <c r="G10" s="4">
-        <v>87.7</v>
+        <v>100</v>
       </c>
       <c r="H10" s="4">
-        <v>92.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
-        <v>83.2</v>
+        <v>99.7</v>
       </c>
       <c r="D11" s="4">
-        <v>70.900000000000006</v>
+        <v>92.5</v>
       </c>
       <c r="E11" s="4">
-        <v>77.3</v>
+        <v>96.2</v>
       </c>
       <c r="F11" s="4">
-        <v>80.900000000000006</v>
+        <v>99.6</v>
       </c>
       <c r="G11" s="4">
-        <v>84</v>
+        <v>98.5</v>
       </c>
       <c r="H11" s="4">
-        <v>125.3</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4">
-        <v>93.7</v>
+        <v>99.7</v>
       </c>
       <c r="D12" s="4">
-        <v>70.099999999999994</v>
+        <v>92.5</v>
       </c>
       <c r="E12" s="4">
-        <v>82.4</v>
+        <v>96.2</v>
       </c>
       <c r="F12" s="4">
-        <v>88.5</v>
+        <v>99.6</v>
       </c>
       <c r="G12" s="4">
-        <v>98.9</v>
+        <v>98.5</v>
       </c>
       <c r="H12" s="4">
-        <v>123.1</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
-        <v>74</v>
+        <v>99.7</v>
       </c>
       <c r="D13" s="4">
-        <v>65.7</v>
+        <v>92.5</v>
       </c>
       <c r="E13" s="4">
-        <v>70</v>
+        <v>96.2</v>
       </c>
       <c r="F13" s="4">
-        <v>70</v>
+        <v>99.6</v>
       </c>
       <c r="G13" s="4">
-        <v>79.400000000000006</v>
+        <v>98.5</v>
       </c>
       <c r="H13" s="4">
-        <v>125.9</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4">
-        <v>102.9</v>
+        <v>99.7</v>
       </c>
       <c r="D14" s="4">
-        <v>62.2</v>
+        <v>92.5</v>
       </c>
       <c r="E14" s="4">
-        <v>83.5</v>
+        <v>96.2</v>
       </c>
       <c r="F14" s="4">
-        <v>112.7</v>
+        <v>99.6</v>
       </c>
       <c r="G14" s="4">
-        <v>83.2</v>
+        <v>98.5</v>
       </c>
       <c r="H14" s="4">
-        <v>77.099999999999994</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4">
-        <v>72.5</v>
+        <v>99.7</v>
       </c>
       <c r="D15" s="4">
-        <v>62</v>
+        <v>92.5</v>
       </c>
       <c r="E15" s="4">
-        <v>67.5</v>
+        <v>96.2</v>
       </c>
       <c r="F15" s="4">
-        <v>69.2</v>
+        <v>99.6</v>
       </c>
       <c r="G15" s="4">
-        <v>80.5</v>
+        <v>98.5</v>
       </c>
       <c r="H15" s="4">
-        <v>118.9</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4">
-        <v>74.900000000000006</v>
+        <v>99.7</v>
       </c>
       <c r="D16" s="4">
-        <v>60.6</v>
+        <v>92.5</v>
       </c>
       <c r="E16" s="4">
-        <v>68.099999999999994</v>
+        <v>96.2</v>
       </c>
       <c r="F16" s="4">
-        <v>68.599999999999994</v>
+        <v>99.6</v>
       </c>
       <c r="G16" s="4">
-        <v>77.900000000000006</v>
+        <v>98.5</v>
       </c>
       <c r="H16" s="4">
-        <v>120.5</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4">
-        <v>81.2</v>
+        <v>111.3</v>
       </c>
       <c r="D17" s="4">
-        <v>60</v>
+        <v>88.8</v>
       </c>
       <c r="E17" s="4">
-        <v>71</v>
+        <v>100.6</v>
       </c>
       <c r="F17" s="4">
-        <v>81</v>
+        <v>117.3</v>
       </c>
       <c r="G17" s="4">
-        <v>74.7</v>
+        <v>115</v>
       </c>
       <c r="H17" s="4">
-        <v>110.2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C18" s="4">
-        <v>79.8</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4">
-        <v>58.3</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E18" s="4">
-        <v>69.5</v>
+        <v>80.2</v>
       </c>
       <c r="F18" s="4">
-        <v>81</v>
+        <v>76.7</v>
       </c>
       <c r="G18" s="4">
-        <v>73.3</v>
+        <v>83</v>
       </c>
       <c r="H18" s="4">
-        <v>111.8</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C19" s="4">
-        <v>79.900000000000006</v>
+        <v>83</v>
       </c>
       <c r="D19" s="4">
-        <v>57.8</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E19" s="4">
-        <v>69.3</v>
+        <v>80.2</v>
       </c>
       <c r="F19" s="4">
-        <v>77.5</v>
+        <v>76.7</v>
       </c>
       <c r="G19" s="4">
-        <v>81.3</v>
+        <v>83</v>
       </c>
       <c r="H19" s="4">
-        <v>129.6</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4">
-        <v>79.8</v>
+        <v>83</v>
       </c>
       <c r="D20" s="4">
-        <v>57.7</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E20" s="4">
-        <v>69.2</v>
+        <v>80.2</v>
       </c>
       <c r="F20" s="4">
-        <v>72.599999999999994</v>
+        <v>76.7</v>
       </c>
       <c r="G20" s="4">
-        <v>79.900000000000006</v>
+        <v>83</v>
       </c>
       <c r="H20" s="4">
-        <v>107.8</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C21" s="4">
-        <v>79.900000000000006</v>
+        <v>83</v>
       </c>
       <c r="D21" s="4">
-        <v>55.5</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E21" s="4">
-        <v>68.2</v>
+        <v>80.2</v>
       </c>
       <c r="F21" s="4">
         <v>76.7</v>
       </c>
       <c r="G21" s="4">
-        <v>72.2</v>
+        <v>83</v>
       </c>
       <c r="H21" s="4">
-        <v>134.5</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C22" s="4">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D22" s="4">
-        <v>53.8</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E22" s="4">
-        <v>65.900000000000006</v>
+        <v>80.2</v>
       </c>
       <c r="F22" s="4">
-        <v>75.3</v>
+        <v>76.7</v>
       </c>
       <c r="G22" s="4">
-        <v>76.900000000000006</v>
+        <v>83</v>
       </c>
       <c r="H22" s="4">
-        <v>136.4</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4">
-        <v>71.8</v>
+        <v>83</v>
       </c>
       <c r="D23" s="4">
-        <v>52.6</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E23" s="4">
-        <v>62.7</v>
+        <v>80.2</v>
       </c>
       <c r="F23" s="4">
-        <v>68.7</v>
+        <v>76.7</v>
       </c>
       <c r="G23" s="4">
-        <v>75.3</v>
+        <v>83</v>
       </c>
       <c r="H23" s="4">
-        <v>128.69999999999999</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C24" s="4">
-        <v>84.5</v>
+        <v>83</v>
       </c>
       <c r="D24" s="4">
-        <v>52.2</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="E24" s="4">
-        <v>69.099999999999994</v>
+        <v>80.2</v>
       </c>
       <c r="F24" s="4">
-        <v>89.1</v>
+        <v>76.7</v>
       </c>
       <c r="G24" s="4">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="H24" s="4">
-        <v>117.2</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4">
-        <v>82.4</v>
+        <v>85.1</v>
       </c>
       <c r="D25" s="4">
-        <v>51.6</v>
+        <v>76</v>
       </c>
       <c r="E25" s="4">
-        <v>67.7</v>
+        <v>80.8</v>
       </c>
       <c r="F25" s="4">
-        <v>81.3</v>
+        <v>83.3</v>
       </c>
       <c r="G25" s="4">
-        <v>74.599999999999994</v>
+        <v>87.5</v>
       </c>
       <c r="H25" s="4">
-        <v>114.1</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4">
-        <v>73.599999999999994</v>
+        <v>85.1</v>
       </c>
       <c r="D26" s="4">
-        <v>51.2</v>
+        <v>76</v>
       </c>
       <c r="E26" s="4">
-        <v>62.9</v>
+        <v>80.8</v>
       </c>
       <c r="F26" s="4">
-        <v>70.400000000000006</v>
+        <v>83.3</v>
       </c>
       <c r="G26" s="4">
-        <v>66.099999999999994</v>
+        <v>87.5</v>
       </c>
       <c r="H26" s="4">
-        <v>129.9</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C27" s="4">
-        <v>74.400000000000006</v>
+        <v>85.1</v>
       </c>
       <c r="D27" s="4">
-        <v>48.8</v>
+        <v>76</v>
       </c>
       <c r="E27" s="4">
-        <v>62.2</v>
+        <v>80.8</v>
       </c>
       <c r="F27" s="4">
-        <v>70.099999999999994</v>
+        <v>83.3</v>
       </c>
       <c r="G27" s="4">
-        <v>77.2</v>
+        <v>87.5</v>
       </c>
       <c r="H27" s="4">
-        <v>138.1</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C28" s="4">
-        <v>79.2</v>
+        <v>85.1</v>
       </c>
       <c r="D28" s="4">
-        <v>48.7</v>
+        <v>76</v>
       </c>
       <c r="E28" s="4">
-        <v>64.599999999999994</v>
+        <v>80.8</v>
       </c>
       <c r="F28" s="4">
-        <v>78.900000000000006</v>
+        <v>83.3</v>
       </c>
       <c r="G28" s="4">
-        <v>76.400000000000006</v>
+        <v>87.5</v>
       </c>
       <c r="H28" s="4">
-        <v>129</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4">
-        <v>75.3</v>
+        <v>85.1</v>
       </c>
       <c r="D29" s="4">
-        <v>47.2</v>
+        <v>76</v>
       </c>
       <c r="E29" s="4">
-        <v>61.9</v>
+        <v>80.8</v>
       </c>
       <c r="F29" s="4">
-        <v>73.7</v>
+        <v>83.3</v>
       </c>
       <c r="G29" s="4">
-        <v>76.400000000000006</v>
+        <v>87.5</v>
       </c>
       <c r="H29" s="4">
-        <v>132.4</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C30" s="4">
-        <v>65.5</v>
+        <v>85.1</v>
       </c>
       <c r="D30" s="4">
-        <v>45.5</v>
+        <v>76</v>
       </c>
       <c r="E30" s="4">
-        <v>55.9</v>
+        <v>80.8</v>
       </c>
       <c r="F30" s="4">
-        <v>63.2</v>
+        <v>83.3</v>
       </c>
       <c r="G30" s="4">
-        <v>69.8</v>
+        <v>87.5</v>
       </c>
       <c r="H30" s="4">
-        <v>130.6</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C31" s="4">
-        <v>74.5</v>
+        <v>85.1</v>
       </c>
       <c r="D31" s="4">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="E31" s="4">
-        <v>60.3</v>
+        <v>80.8</v>
       </c>
       <c r="F31" s="4">
-        <v>75.400000000000006</v>
+        <v>83.3</v>
       </c>
       <c r="G31" s="4">
-        <v>68</v>
+        <v>87.5</v>
       </c>
       <c r="H31" s="4">
-        <v>138.1</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C32" s="4">
-        <v>71.7</v>
+        <v>94</v>
       </c>
       <c r="D32" s="4">
-        <v>45</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="E32" s="4">
-        <v>58.9</v>
+        <v>84.7</v>
       </c>
       <c r="F32" s="4">
-        <v>70.400000000000006</v>
+        <v>96.7</v>
       </c>
       <c r="G32" s="4">
-        <v>72.599999999999994</v>
+        <v>85.5</v>
       </c>
       <c r="H32" s="4">
-        <v>88.6</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C33" s="4">
-        <v>80.7</v>
+        <v>79.2</v>
       </c>
       <c r="D33" s="4">
-        <v>44.8</v>
+        <v>73.8</v>
       </c>
       <c r="E33" s="4">
-        <v>63.6</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F33" s="4">
-        <v>79.900000000000006</v>
+        <v>76</v>
       </c>
       <c r="G33" s="4">
-        <v>79.7</v>
+        <v>88.7</v>
       </c>
       <c r="H33" s="4">
-        <v>94.7</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C34" s="4">
-        <v>69.5</v>
+        <v>79.2</v>
       </c>
       <c r="D34" s="4">
-        <v>44.7</v>
+        <v>73.8</v>
       </c>
       <c r="E34" s="4">
-        <v>57.6</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F34" s="4">
-        <v>62.9</v>
+        <v>76</v>
       </c>
       <c r="G34" s="4">
-        <v>72.3</v>
+        <v>88.7</v>
       </c>
       <c r="H34" s="4">
-        <v>151.6</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C35" s="4">
-        <v>69.900000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="D35" s="4">
-        <v>44</v>
+        <v>73.8</v>
       </c>
       <c r="E35" s="4">
-        <v>57.5</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F35" s="4">
-        <v>64.599999999999994</v>
+        <v>76</v>
       </c>
       <c r="G35" s="4">
-        <v>65.7</v>
+        <v>88.7</v>
       </c>
       <c r="H35" s="4">
-        <v>86.6</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C36" s="4">
-        <v>71.900000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="D36" s="4">
-        <v>43.5</v>
+        <v>73.8</v>
       </c>
       <c r="E36" s="4">
-        <v>58.3</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F36" s="4">
-        <v>70.3</v>
+        <v>76</v>
       </c>
       <c r="G36" s="4">
-        <v>67</v>
+        <v>88.7</v>
       </c>
       <c r="H36" s="4">
-        <v>94.9</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C37" s="4">
-        <v>74.900000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="D37" s="4">
-        <v>42.7</v>
+        <v>73.8</v>
       </c>
       <c r="E37" s="4">
-        <v>59.5</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F37" s="4">
-        <v>78.400000000000006</v>
+        <v>76</v>
       </c>
       <c r="G37" s="4">
-        <v>62.7</v>
+        <v>88.7</v>
       </c>
       <c r="H37" s="4">
-        <v>125.5</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C38" s="4">
-        <v>69.400000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="D38" s="4">
-        <v>42.3</v>
+        <v>73.8</v>
       </c>
       <c r="E38" s="4">
-        <v>56.4</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F38" s="4">
-        <v>66.8</v>
+        <v>76</v>
       </c>
       <c r="G38" s="4">
-        <v>64.8</v>
+        <v>88.7</v>
       </c>
       <c r="H38" s="4">
-        <v>152.19999999999999</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C39" s="4">
-        <v>72.400000000000006</v>
+        <v>85</v>
       </c>
       <c r="D39" s="4">
-        <v>42.3</v>
+        <v>73</v>
       </c>
       <c r="E39" s="4">
-        <v>58</v>
+        <v>79.3</v>
       </c>
       <c r="F39" s="4">
-        <v>66.3</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="G39" s="4">
-        <v>74</v>
+        <v>83.8</v>
       </c>
       <c r="H39" s="4">
-        <v>103</v>
+        <v>143.6</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4">
-        <v>70.400000000000006</v>
+        <v>85</v>
       </c>
       <c r="D40" s="4">
-        <v>41.9</v>
+        <v>73</v>
       </c>
       <c r="E40" s="4">
-        <v>56.8</v>
+        <v>79.3</v>
       </c>
       <c r="F40" s="4">
-        <v>64.599999999999994</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="G40" s="4">
-        <v>71.2</v>
+        <v>83.8</v>
       </c>
       <c r="H40" s="4">
-        <v>117.4</v>
+        <v>143.6</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C41" s="4">
-        <v>73.400000000000006</v>
+        <v>85</v>
       </c>
       <c r="D41" s="4">
-        <v>41.8</v>
+        <v>73</v>
       </c>
       <c r="E41" s="4">
-        <v>58.3</v>
+        <v>79.3</v>
       </c>
       <c r="F41" s="4">
-        <v>73.900000000000006</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="G41" s="4">
-        <v>64.3</v>
+        <v>83.8</v>
       </c>
       <c r="H41" s="4">
-        <v>138</v>
+        <v>143.6</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C42" s="4">
-        <v>67.099999999999994</v>
+        <v>85</v>
       </c>
       <c r="D42" s="4">
-        <v>41.5</v>
+        <v>73</v>
       </c>
       <c r="E42" s="4">
-        <v>54.9</v>
+        <v>79.3</v>
       </c>
       <c r="F42" s="4">
-        <v>59.8</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="G42" s="4">
-        <v>69</v>
+        <v>83.8</v>
       </c>
       <c r="H42" s="4">
-        <v>138</v>
+        <v>143.6</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4">
-        <v>73.3</v>
+        <v>81.2</v>
       </c>
       <c r="D43" s="4">
-        <v>41.4</v>
+        <v>71.2</v>
       </c>
       <c r="E43" s="4">
-        <v>58.1</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="F43" s="4">
-        <v>66.5</v>
+        <v>79.5</v>
       </c>
       <c r="G43" s="4">
-        <v>72.5</v>
+        <v>87.7</v>
       </c>
       <c r="H43" s="4">
-        <v>115.5</v>
+        <v>92.9</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C44" s="4">
-        <v>72.7</v>
+        <v>83.2</v>
       </c>
       <c r="D44" s="4">
-        <v>41.3</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="E44" s="4">
-        <v>57.6</v>
+        <v>77.3</v>
       </c>
       <c r="F44" s="4">
-        <v>66.3</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="G44" s="4">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="H44" s="4">
-        <v>122</v>
+        <v>125.3</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C45" s="4">
-        <v>85.4</v>
+        <v>93.7</v>
       </c>
       <c r="D45" s="4">
-        <v>41</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E45" s="4">
-        <v>64.2</v>
+        <v>82.4</v>
       </c>
       <c r="F45" s="4">
-        <v>87.5</v>
+        <v>88.5</v>
       </c>
       <c r="G45" s="4">
-        <v>77.900000000000006</v>
+        <v>98.9</v>
       </c>
       <c r="H45" s="4">
-        <v>114.9</v>
+        <v>123.1</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C46" s="4">
-        <v>69.099999999999994</v>
+        <v>74</v>
       </c>
       <c r="D46" s="4">
-        <v>40.4</v>
+        <v>65.7</v>
       </c>
       <c r="E46" s="4">
-        <v>55.3</v>
+        <v>70</v>
       </c>
       <c r="F46" s="4">
-        <v>70.900000000000006</v>
+        <v>70</v>
       </c>
       <c r="G46" s="4">
-        <v>70.8</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="H46" s="4">
-        <v>136.30000000000001</v>
+        <v>125.9</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C47" s="4">
-        <v>75.599999999999994</v>
+        <v>102.9</v>
       </c>
       <c r="D47" s="4">
-        <v>39.9</v>
+        <v>62.2</v>
       </c>
       <c r="E47" s="4">
-        <v>58.5</v>
+        <v>83.5</v>
       </c>
       <c r="F47" s="4">
-        <v>75.8</v>
+        <v>112.7</v>
       </c>
       <c r="G47" s="4">
-        <v>67.900000000000006</v>
+        <v>83.2</v>
       </c>
       <c r="H47" s="4">
-        <v>128.30000000000001</v>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C48" s="4">
-        <v>70.8</v>
+        <v>72.5</v>
       </c>
       <c r="D48" s="4">
-        <v>39.6</v>
+        <v>62</v>
       </c>
       <c r="E48" s="4">
-        <v>55.9</v>
+        <v>67.5</v>
       </c>
       <c r="F48" s="4">
-        <v>62.9</v>
+        <v>69.2</v>
       </c>
       <c r="G48" s="4">
-        <v>67</v>
+        <v>80.5</v>
       </c>
       <c r="H48" s="4">
-        <v>148.1</v>
+        <v>118.9</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C49" s="4">
-        <v>63.2</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="D49" s="4">
-        <v>39.5</v>
+        <v>60.6</v>
       </c>
       <c r="E49" s="4">
-        <v>51.9</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="F49" s="4">
-        <v>63.3</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="G49" s="4">
-        <v>58.8</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="H49" s="4">
-        <v>116.5</v>
+        <v>120.5</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C50" s="4">
-        <v>65.8</v>
+        <v>81.2</v>
       </c>
       <c r="D50" s="4">
-        <v>39.5</v>
+        <v>60</v>
       </c>
       <c r="E50" s="4">
-        <v>53.2</v>
+        <v>71</v>
       </c>
       <c r="F50" s="4">
-        <v>59.8</v>
+        <v>81</v>
       </c>
       <c r="G50" s="4">
-        <v>80.599999999999994</v>
+        <v>74.7</v>
       </c>
       <c r="H50" s="4">
-        <v>198</v>
+        <v>110.2</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C51" s="4">
-        <v>75.400000000000006</v>
+        <v>79.8</v>
       </c>
       <c r="D51" s="4">
-        <v>39</v>
+        <v>58.3</v>
       </c>
       <c r="E51" s="4">
-        <v>58</v>
+        <v>69.5</v>
       </c>
       <c r="F51" s="4">
-        <v>75.400000000000006</v>
+        <v>81</v>
       </c>
       <c r="G51" s="4">
-        <v>68.2</v>
+        <v>73.3</v>
       </c>
       <c r="H51" s="4">
-        <v>129.80000000000001</v>
+        <v>111.8</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C52" s="4">
-        <v>77.900000000000006</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D52" s="4">
-        <v>38.4</v>
+        <v>57.8</v>
       </c>
       <c r="E52" s="4">
-        <v>59</v>
+        <v>69.3</v>
       </c>
       <c r="F52" s="4">
-        <v>78.099999999999994</v>
+        <v>77.5</v>
       </c>
       <c r="G52" s="4">
-        <v>69.7</v>
+        <v>81.3</v>
       </c>
       <c r="H52" s="4">
-        <v>107.4</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C53" s="4">
-        <v>75.900000000000006</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D53" s="4">
-        <v>38.200000000000003</v>
+        <v>57.8</v>
       </c>
       <c r="E53" s="4">
-        <v>57.9</v>
+        <v>69.3</v>
       </c>
       <c r="F53" s="4">
-        <v>80.900000000000006</v>
+        <v>77.5</v>
       </c>
       <c r="G53" s="4">
-        <v>62.9</v>
+        <v>81.3</v>
       </c>
       <c r="H53" s="4">
-        <v>122.9</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C54" s="4">
-        <v>73</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D54" s="4">
-        <v>38.1</v>
+        <v>57.8</v>
       </c>
       <c r="E54" s="4">
-        <v>56.3</v>
+        <v>69.3</v>
       </c>
       <c r="F54" s="4">
-        <v>69.7</v>
+        <v>77.5</v>
       </c>
       <c r="G54" s="4">
-        <v>77.599999999999994</v>
+        <v>81.3</v>
       </c>
       <c r="H54" s="4">
-        <v>131.6</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C55" s="4">
-        <v>73.099999999999994</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D55" s="4">
-        <v>37.700000000000003</v>
+        <v>57.8</v>
       </c>
       <c r="E55" s="4">
-        <v>56.2</v>
+        <v>69.3</v>
       </c>
       <c r="F55" s="4">
-        <v>69</v>
+        <v>77.5</v>
       </c>
       <c r="G55" s="4">
-        <v>69.8</v>
+        <v>81.3</v>
       </c>
       <c r="H55" s="4">
-        <v>124.5</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="C56" s="4">
-        <v>72.400000000000006</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D56" s="4">
-        <v>37.700000000000003</v>
+        <v>57.8</v>
       </c>
       <c r="E56" s="4">
-        <v>55.8</v>
+        <v>69.3</v>
       </c>
       <c r="F56" s="4">
-        <v>70.5</v>
+        <v>77.5</v>
       </c>
       <c r="G56" s="4">
-        <v>57.2</v>
+        <v>81.3</v>
       </c>
       <c r="H56" s="4">
-        <v>95.2</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C57" s="4">
-        <v>75.3</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D57" s="4">
-        <v>37.299999999999997</v>
+        <v>57.8</v>
       </c>
       <c r="E57" s="4">
-        <v>57.1</v>
+        <v>69.3</v>
       </c>
       <c r="F57" s="4">
-        <v>80.3</v>
+        <v>77.5</v>
       </c>
       <c r="G57" s="4">
-        <v>66.3</v>
+        <v>81.3</v>
       </c>
       <c r="H57" s="4">
-        <v>83.6</v>
+        <v>129.6</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C58" s="4">
-        <v>74.400000000000006</v>
+        <v>79.8</v>
       </c>
       <c r="D58" s="4">
-        <v>37.200000000000003</v>
+        <v>57.7</v>
       </c>
       <c r="E58" s="4">
-        <v>56.6</v>
+        <v>69.2</v>
       </c>
       <c r="F58" s="4">
-        <v>73.7</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="G58" s="4">
-        <v>73.2</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="H58" s="4">
-        <v>131.9</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C59" s="4">
-        <v>72.5</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="D59" s="4">
-        <v>37.1</v>
+        <v>55.5</v>
       </c>
       <c r="E59" s="4">
-        <v>55.6</v>
+        <v>68.2</v>
       </c>
       <c r="F59" s="4">
-        <v>68.8</v>
+        <v>76.7</v>
       </c>
       <c r="G59" s="4">
-        <v>63.4</v>
+        <v>72.2</v>
       </c>
       <c r="H59" s="4">
-        <v>117.8</v>
+        <v>134.5</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C60" s="4">
-        <v>72.599999999999994</v>
+        <v>77</v>
       </c>
       <c r="D60" s="4">
-        <v>37.1</v>
+        <v>53.8</v>
       </c>
       <c r="E60" s="4">
-        <v>55.6</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="F60" s="4">
-        <v>72.400000000000006</v>
+        <v>75.3</v>
       </c>
       <c r="G60" s="4">
-        <v>66.599999999999994</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="H60" s="4">
-        <v>121.4</v>
+        <v>136.4</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C61" s="4">
-        <v>64.8</v>
+        <v>77</v>
       </c>
       <c r="D61" s="4">
-        <v>36.1</v>
+        <v>53.8</v>
       </c>
       <c r="E61" s="4">
-        <v>51.1</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="F61" s="4">
-        <v>64.8</v>
+        <v>75.3</v>
       </c>
       <c r="G61" s="4">
-        <v>65</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="H61" s="4">
-        <v>156.5</v>
+        <v>136.4</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C62" s="4">
-        <v>60.8</v>
+        <v>77</v>
       </c>
       <c r="D62" s="4">
-        <v>35.200000000000003</v>
+        <v>53.8</v>
       </c>
       <c r="E62" s="4">
-        <v>48.5</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="F62" s="4">
-        <v>56.9</v>
+        <v>75.3</v>
       </c>
       <c r="G62" s="4">
-        <v>58.6</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="H62" s="4">
-        <v>146.9</v>
+        <v>136.4</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C63" s="4">
-        <v>67.7</v>
+        <v>77</v>
       </c>
       <c r="D63" s="4">
-        <v>34.4</v>
+        <v>53.8</v>
       </c>
       <c r="E63" s="4">
-        <v>51.7</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="F63" s="4">
-        <v>68.099999999999994</v>
+        <v>75.3</v>
       </c>
       <c r="G63" s="4">
-        <v>64.2</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="H63" s="4">
-        <v>104.9</v>
+        <v>136.4</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="C64" s="4">
-        <v>65.8</v>
+        <v>71.8</v>
       </c>
       <c r="D64" s="4">
-        <v>32.299999999999997</v>
+        <v>52.6</v>
       </c>
       <c r="E64" s="4">
-        <v>49.8</v>
+        <v>62.7</v>
       </c>
       <c r="F64" s="4">
-        <v>64.3</v>
+        <v>68.7</v>
       </c>
       <c r="G64" s="4">
-        <v>61.9</v>
+        <v>75.3</v>
       </c>
       <c r="H64" s="4">
-        <v>175.6</v>
+        <v>128.69999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="C65" s="4">
-        <v>67.2</v>
+        <v>84.5</v>
       </c>
       <c r="D65" s="4">
-        <v>31.9</v>
+        <v>52.2</v>
       </c>
       <c r="E65" s="4">
-        <v>50.3</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="F65" s="4">
-        <v>67.8</v>
+        <v>89.1</v>
       </c>
       <c r="G65" s="4">
-        <v>63.9</v>
+        <v>73</v>
       </c>
       <c r="H65" s="4">
-        <v>155.9</v>
+        <v>117.2</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C66" s="4">
-        <v>76.099999999999994</v>
+        <v>82.4</v>
       </c>
       <c r="D66" s="4">
-        <v>30.9</v>
+        <v>51.6</v>
       </c>
       <c r="E66" s="4">
-        <v>54.5</v>
+        <v>67.7</v>
       </c>
       <c r="F66" s="4">
-        <v>70.2</v>
+        <v>81.3</v>
       </c>
       <c r="G66" s="4">
-        <v>78.8</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="H66" s="4">
-        <v>115.3</v>
+        <v>114.1</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
+        <v>25</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="4">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D67" s="4">
+        <v>51.2</v>
+      </c>
+      <c r="E67" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="F67" s="4">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="G67" s="4">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="H67" s="4">
+        <v>129.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>26</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D68" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="E68" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="F68" s="4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G68" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="H68" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>26</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D69" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="E69" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="F69" s="4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G69" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="H69" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <v>26</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D70" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="E70" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="F70" s="4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G70" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="H70" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>26</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D71" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="E71" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="F71" s="4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G71" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="H71" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>26</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D72" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="E72" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="F72" s="4">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G72" s="4">
+        <v>77.2</v>
+      </c>
+      <c r="H72" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>27</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D73" s="4">
+        <v>48.7</v>
+      </c>
+      <c r="E73" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F73" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="G73" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H73" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>27</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D74" s="4">
+        <v>48.7</v>
+      </c>
+      <c r="E74" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F74" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="G74" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H74" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>27</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D75" s="4">
+        <v>48.7</v>
+      </c>
+      <c r="E75" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F75" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="G75" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H75" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>27</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D76" s="4">
+        <v>48.7</v>
+      </c>
+      <c r="E76" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F76" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="G76" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H76" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>27</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="4">
+        <v>79.2</v>
+      </c>
+      <c r="D77" s="4">
+        <v>48.7</v>
+      </c>
+      <c r="E77" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F77" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="G77" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H77" s="4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>28</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="4">
+        <v>75.3</v>
+      </c>
+      <c r="D78" s="4">
+        <v>47.2</v>
+      </c>
+      <c r="E78" s="4">
+        <v>61.9</v>
+      </c>
+      <c r="F78" s="4">
+        <v>73.7</v>
+      </c>
+      <c r="G78" s="4">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H78" s="4">
+        <v>132.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>29</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="4">
+        <v>65.5</v>
+      </c>
+      <c r="D79" s="4">
+        <v>45.5</v>
+      </c>
+      <c r="E79" s="4">
+        <v>55.9</v>
+      </c>
+      <c r="F79" s="4">
+        <v>63.2</v>
+      </c>
+      <c r="G79" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="H79" s="4">
+        <v>130.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>30</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="4">
+        <v>74.5</v>
+      </c>
+      <c r="D80" s="4">
+        <v>45</v>
+      </c>
+      <c r="E80" s="4">
+        <v>60.3</v>
+      </c>
+      <c r="F80" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="G80" s="4">
+        <v>68</v>
+      </c>
+      <c r="H80" s="4">
+        <v>138.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>31</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="4">
+        <v>45</v>
+      </c>
+      <c r="E81" s="4">
+        <v>58.9</v>
+      </c>
+      <c r="F81" s="4">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="G81" s="4">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="H81" s="4">
+        <v>88.6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>32</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="4">
+        <v>80.7</v>
+      </c>
+      <c r="D82" s="4">
+        <v>44.8</v>
+      </c>
+      <c r="E82" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="F82" s="4">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="G82" s="4">
+        <v>79.7</v>
+      </c>
+      <c r="H82" s="4">
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>28</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D83" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E83" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F83" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G83" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H83" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>29</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D84" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E84" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F84" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G84" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H84" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>30</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D85" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E85" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F85" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G85" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H85" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>31</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D86" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E86" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F86" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G86" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H86" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>32</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D87" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E87" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F87" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G87" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H87" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>33</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="4">
+        <v>69.5</v>
+      </c>
+      <c r="D88" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="E88" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F88" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G88" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H88" s="4">
+        <v>151.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>34</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="4">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="D89" s="4">
+        <v>44</v>
+      </c>
+      <c r="E89" s="4">
+        <v>57.5</v>
+      </c>
+      <c r="F89" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G89" s="4">
+        <v>65.7</v>
+      </c>
+      <c r="H89" s="4">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>35</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C90" s="4">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D90" s="4">
+        <v>43.5</v>
+      </c>
+      <c r="E90" s="4">
+        <v>58.3</v>
+      </c>
+      <c r="F90" s="4">
+        <v>70.3</v>
+      </c>
+      <c r="G90" s="4">
+        <v>67</v>
+      </c>
+      <c r="H90" s="4">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>36</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C91" s="4">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="D91" s="4">
+        <v>42.7</v>
+      </c>
+      <c r="E91" s="4">
+        <v>59.5</v>
+      </c>
+      <c r="F91" s="4">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="G91" s="4">
+        <v>62.7</v>
+      </c>
+      <c r="H91" s="4">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>37</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="4">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="D92" s="4">
+        <v>42.3</v>
+      </c>
+      <c r="E92" s="4">
+        <v>56.4</v>
+      </c>
+      <c r="F92" s="4">
+        <v>66.8</v>
+      </c>
+      <c r="G92" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="H92" s="4">
+        <v>152.19999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>38</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" s="4">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D93" s="4">
+        <v>42.3</v>
+      </c>
+      <c r="E93" s="4">
+        <v>58</v>
+      </c>
+      <c r="F93" s="4">
+        <v>66.3</v>
+      </c>
+      <c r="G93" s="4">
+        <v>74</v>
+      </c>
+      <c r="H93" s="4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>39</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" s="4">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="D94" s="4">
+        <v>41.9</v>
+      </c>
+      <c r="E94" s="4">
+        <v>56.8</v>
+      </c>
+      <c r="F94" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G94" s="4">
+        <v>71.2</v>
+      </c>
+      <c r="H94" s="4">
+        <v>117.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>40</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C95" s="4">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="D95" s="4">
+        <v>41.8</v>
+      </c>
+      <c r="E95" s="4">
+        <v>58.3</v>
+      </c>
+      <c r="F95" s="4">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G95" s="4">
+        <v>64.3</v>
+      </c>
+      <c r="H95" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>41</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C96" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D96" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="E96" s="4">
+        <v>54.9</v>
+      </c>
+      <c r="F96" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G96" s="4">
+        <v>69</v>
+      </c>
+      <c r="H96" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>41</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D97" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="E97" s="4">
+        <v>54.9</v>
+      </c>
+      <c r="F97" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G97" s="4">
+        <v>69</v>
+      </c>
+      <c r="H97" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <v>41</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C98" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D98" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="E98" s="4">
+        <v>54.9</v>
+      </c>
+      <c r="F98" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G98" s="4">
+        <v>69</v>
+      </c>
+      <c r="H98" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <v>41</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C99" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D99" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="E99" s="4">
+        <v>54.9</v>
+      </c>
+      <c r="F99" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G99" s="4">
+        <v>69</v>
+      </c>
+      <c r="H99" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>41</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C100" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D100" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="E100" s="4">
+        <v>54.9</v>
+      </c>
+      <c r="F100" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G100" s="4">
+        <v>69</v>
+      </c>
+      <c r="H100" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A101" s="4">
+        <v>42</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" s="4">
+        <v>73.3</v>
+      </c>
+      <c r="D101" s="4">
+        <v>41.4</v>
+      </c>
+      <c r="E101" s="4">
+        <v>58.1</v>
+      </c>
+      <c r="F101" s="4">
+        <v>66.5</v>
+      </c>
+      <c r="G101" s="4">
+        <v>72.5</v>
+      </c>
+      <c r="H101" s="4">
+        <v>115.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A102" s="4">
+        <v>43</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C102" s="4">
+        <v>72.7</v>
+      </c>
+      <c r="D102" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="E102" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="F102" s="4">
+        <v>66.3</v>
+      </c>
+      <c r="G102" s="4">
+        <v>67</v>
+      </c>
+      <c r="H102" s="4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A103" s="4">
+        <v>44</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" s="4">
+        <v>85.4</v>
+      </c>
+      <c r="D103" s="4">
+        <v>41</v>
+      </c>
+      <c r="E103" s="4">
+        <v>64.2</v>
+      </c>
+      <c r="F103" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="G103" s="4">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="H103" s="4">
+        <v>114.9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A104" s="4">
+        <v>45</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="D104" s="4">
+        <v>40.4</v>
+      </c>
+      <c r="E104" s="4">
+        <v>55.3</v>
+      </c>
+      <c r="F104" s="4">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="G104" s="4">
+        <v>70.8</v>
+      </c>
+      <c r="H104" s="4">
+        <v>136.30000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A105" s="4">
+        <v>46</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C105" s="4">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="D105" s="4">
+        <v>39.9</v>
+      </c>
+      <c r="E105" s="4">
+        <v>58.5</v>
+      </c>
+      <c r="F105" s="4">
+        <v>75.8</v>
+      </c>
+      <c r="G105" s="4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="H105" s="4">
+        <v>128.30000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A106" s="4">
+        <v>47</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C106" s="4">
+        <v>70.8</v>
+      </c>
+      <c r="D106" s="4">
+        <v>39.6</v>
+      </c>
+      <c r="E106" s="4">
+        <v>55.9</v>
+      </c>
+      <c r="F106" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="G106" s="4">
+        <v>67</v>
+      </c>
+      <c r="H106" s="4">
+        <v>148.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A107" s="4">
+        <v>48</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" s="4">
+        <v>63.2</v>
+      </c>
+      <c r="D107" s="4">
+        <v>39.5</v>
+      </c>
+      <c r="E107" s="4">
+        <v>51.9</v>
+      </c>
+      <c r="F107" s="4">
+        <v>63.3</v>
+      </c>
+      <c r="G107" s="4">
+        <v>58.8</v>
+      </c>
+      <c r="H107" s="4">
+        <v>116.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A108" s="4">
+        <v>49</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C108" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="D108" s="4">
+        <v>39.5</v>
+      </c>
+      <c r="E108" s="4">
+        <v>53.2</v>
+      </c>
+      <c r="F108" s="4">
+        <v>59.8</v>
+      </c>
+      <c r="G108" s="4">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="H108" s="4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A109" s="4">
+        <v>50</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C109" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D109" s="4">
+        <v>39</v>
+      </c>
+      <c r="E109" s="4">
+        <v>58</v>
+      </c>
+      <c r="F109" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="G109" s="4">
+        <v>68.2</v>
+      </c>
+      <c r="H109" s="4">
+        <v>129.80000000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A110" s="4">
+        <v>51</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C110" s="4">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="D110" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="E110" s="4">
+        <v>59</v>
+      </c>
+      <c r="F110" s="4">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="G110" s="4">
+        <v>69.7</v>
+      </c>
+      <c r="H110" s="4">
+        <v>107.4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A111" s="4">
+        <v>52</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C111" s="4">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="D111" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E111" s="4">
+        <v>57.9</v>
+      </c>
+      <c r="F111" s="4">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="G111" s="4">
+        <v>62.9</v>
+      </c>
+      <c r="H111" s="4">
+        <v>122.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A112" s="4">
+        <v>53</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C112" s="4">
+        <v>73</v>
+      </c>
+      <c r="D112" s="4">
+        <v>38.1</v>
+      </c>
+      <c r="E112" s="4">
+        <v>56.3</v>
+      </c>
+      <c r="F112" s="4">
+        <v>69.7</v>
+      </c>
+      <c r="G112" s="4">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="H112" s="4">
+        <v>131.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A113" s="4">
+        <v>54</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C113" s="4">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="D113" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E113" s="4">
+        <v>56.2</v>
+      </c>
+      <c r="F113" s="4">
+        <v>69</v>
+      </c>
+      <c r="G113" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="H113" s="4">
+        <v>124.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A114" s="4">
+        <v>55</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C114" s="4">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D114" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E114" s="4">
+        <v>55.8</v>
+      </c>
+      <c r="F114" s="4">
+        <v>70.5</v>
+      </c>
+      <c r="G114" s="4">
+        <v>57.2</v>
+      </c>
+      <c r="H114" s="4">
+        <v>95.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A115" s="4">
+        <v>56</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" s="4">
+        <v>75.3</v>
+      </c>
+      <c r="D115" s="4">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="E115" s="4">
+        <v>57.1</v>
+      </c>
+      <c r="F115" s="4">
+        <v>80.3</v>
+      </c>
+      <c r="G115" s="4">
+        <v>66.3</v>
+      </c>
+      <c r="H115" s="4">
+        <v>83.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A116" s="4">
+        <v>57</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D116" s="4">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E116" s="4">
+        <v>56.6</v>
+      </c>
+      <c r="F116" s="4">
+        <v>73.7</v>
+      </c>
+      <c r="G116" s="4">
+        <v>73.2</v>
+      </c>
+      <c r="H116" s="4">
+        <v>131.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A117" s="4">
+        <v>58</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C117" s="4">
+        <v>72.5</v>
+      </c>
+      <c r="D117" s="4">
+        <v>37.1</v>
+      </c>
+      <c r="E117" s="4">
+        <v>55.6</v>
+      </c>
+      <c r="F117" s="4">
+        <v>68.8</v>
+      </c>
+      <c r="G117" s="4">
+        <v>63.4</v>
+      </c>
+      <c r="H117" s="4">
+        <v>117.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A118" s="4">
+        <v>59</v>
+      </c>
+      <c r="B118" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C118" s="4">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="D118" s="4">
+        <v>37.1</v>
+      </c>
+      <c r="E118" s="4">
+        <v>55.6</v>
+      </c>
+      <c r="F118" s="4">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="G118" s="4">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="H118" s="4">
+        <v>121.4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A119" s="4">
+        <v>60</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C119" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="D119" s="4">
+        <v>36.1</v>
+      </c>
+      <c r="E119" s="4">
+        <v>51.1</v>
+      </c>
+      <c r="F119" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="G119" s="4">
+        <v>65</v>
+      </c>
+      <c r="H119" s="4">
+        <v>156.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A120" s="4">
+        <v>61</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" s="4">
+        <v>60.8</v>
+      </c>
+      <c r="D120" s="4">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E120" s="4">
+        <v>48.5</v>
+      </c>
+      <c r="F120" s="4">
+        <v>56.9</v>
+      </c>
+      <c r="G120" s="4">
+        <v>58.6</v>
+      </c>
+      <c r="H120" s="4">
+        <v>146.9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A121" s="4">
+        <v>62</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C121" s="4">
+        <v>67.7</v>
+      </c>
+      <c r="D121" s="4">
+        <v>34.4</v>
+      </c>
+      <c r="E121" s="4">
+        <v>51.7</v>
+      </c>
+      <c r="F121" s="4">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="G121" s="4">
+        <v>64.2</v>
+      </c>
+      <c r="H121" s="4">
+        <v>104.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A122" s="4">
+        <v>63</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C122" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="D122" s="4">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E122" s="4">
+        <v>49.8</v>
+      </c>
+      <c r="F122" s="4">
+        <v>64.3</v>
+      </c>
+      <c r="G122" s="4">
+        <v>61.9</v>
+      </c>
+      <c r="H122" s="4">
+        <v>175.6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A123" s="4">
+        <v>64</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C123" s="4">
+        <v>67.2</v>
+      </c>
+      <c r="D123" s="4">
+        <v>31.9</v>
+      </c>
+      <c r="E123" s="4">
+        <v>50.3</v>
+      </c>
+      <c r="F123" s="4">
+        <v>67.8</v>
+      </c>
+      <c r="G123" s="4">
+        <v>63.9</v>
+      </c>
+      <c r="H123" s="4">
+        <v>155.9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A124" s="4">
+        <v>65</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C124" s="4">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="D124" s="4">
+        <v>30.9</v>
+      </c>
+      <c r="E124" s="4">
+        <v>54.5</v>
+      </c>
+      <c r="F124" s="4">
+        <v>70.2</v>
+      </c>
+      <c r="G124" s="4">
+        <v>78.8</v>
+      </c>
+      <c r="H124" s="4">
+        <v>115.3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A125" s="4">
+        <v>66</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C125" s="4">
         <v>64.3</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D125" s="4">
         <v>30.3</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E125" s="4">
         <v>48</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F125" s="4">
         <v>60.1</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G125" s="4">
         <v>54.4</v>
       </c>
-      <c r="H67" s="4">
+      <c r="H125" s="4">
         <v>174.9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{505D81DA-7DA7-0E4B-A961-407D8CB180A3}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.numbeo.com/cost-of-living/in/San-Francisco" xr:uid="{3F107AE5-F588-4944-BA28-93A8FE0416B4}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.numbeo.com/cost-of-living/in/Santa-Barbara" xr:uid="{6DCAC14C-23FC-4D43-99A6-13D9E84477BB}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{1FC5B719-FC20-D140-B454-667BEE99C9DC}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{6B5E2C07-E151-2746-8E87-D24F70A057D5}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.numbeo.com/cost-of-living/in/Oakland" xr:uid="{10B6EAF1-FC05-5E4C-A743-0F06A842424D}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{658DCA8E-5C0E-224C-B78E-6CAC1EFE822B}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.numbeo.com/cost-of-living/in/San-Jose" xr:uid="{4EE70F74-3CAC-0142-BCBD-48A3717DD8DE}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.numbeo.com/cost-of-living/in/Miami" xr:uid="{96B2F11C-5318-8E40-9210-5DE462401878}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.numbeo.com/cost-of-living/in/Washington" xr:uid="{03E1A461-C305-154B-956F-104282382F8B}"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://www.numbeo.com/cost-of-living/in/Seattle" xr:uid="{6DF47F8F-61E9-CC44-A05F-579FE4701E42}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://www.numbeo.com/cost-of-living/in/Austin" xr:uid="{D99D0BFA-6C8E-4C40-9D09-B1D990C9FE49}"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://www.numbeo.com/cost-of-living/in/Honolulu" xr:uid="{ABEF44A0-E25D-4C4D-B6DC-1803D593880E}"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://www.numbeo.com/cost-of-living/in/Fort-Lauderdale" xr:uid="{CCFDCB0A-15E2-1F4D-87A9-CA749F786BB4}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://www.numbeo.com/cost-of-living/in/Tampa" xr:uid="{3D2101C6-1467-A24A-816D-D3E8047DB0DC}"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://www.numbeo.com/cost-of-living/in/Charlotte" xr:uid="{478C7A11-1CA6-994D-9DE8-BD796B6DCC5A}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://www.numbeo.com/cost-of-living/in/Nashville" xr:uid="{705067BF-7B15-CA41-BA04-463A11DEED40}"/>
-    <hyperlink ref="B19" r:id="rId18" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{CFE3C87A-8C65-8741-9256-67BD8EBBA557}"/>
-    <hyperlink ref="B20" r:id="rId19" display="https://www.numbeo.com/cost-of-living/in/Raleigh" xr:uid="{CD55AD67-D73F-834F-87A8-7F56A6463E1F}"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://www.numbeo.com/cost-of-living/in/Denver" xr:uid="{79516C99-3676-F64F-83C3-A0D706BF5810}"/>
-    <hyperlink ref="B22" r:id="rId21" display="https://www.numbeo.com/cost-of-living/in/Dallas" xr:uid="{D3F59C0C-85A4-5642-B16F-A7E4B0250235}"/>
-    <hyperlink ref="B23" r:id="rId22" display="https://www.numbeo.com/cost-of-living/in/Orlando" xr:uid="{A28F9486-B396-DC4E-8945-DA1E1A7DEEC9}"/>
-    <hyperlink ref="B24" r:id="rId23" display="https://www.numbeo.com/cost-of-living/in/Sacramento" xr:uid="{AF06AE15-18CC-9A4C-A02A-5C2FFC62F127}"/>
-    <hyperlink ref="B25" r:id="rId24" display="https://www.numbeo.com/cost-of-living/in/Portland" xr:uid="{0719E6BF-CB4D-5947-B6F7-A1B3F682B57E}"/>
-    <hyperlink ref="B26" r:id="rId25" display="https://www.numbeo.com/cost-of-living/in/Atlanta" xr:uid="{9BD28DCF-8FA3-3846-8D35-F823EA1E93C0}"/>
-    <hyperlink ref="B27" r:id="rId26" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{017C6336-EC6C-854A-AA66-C8BF857CD35A}"/>
-    <hyperlink ref="B28" r:id="rId27" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{FC88C82F-4832-BA44-97A5-A27FBD0F376B}"/>
-    <hyperlink ref="B29" r:id="rId28" display="https://www.numbeo.com/cost-of-living/in/Minneapolis" xr:uid="{C2DC497A-EF35-AF4A-97E3-4060F7E40377}"/>
-    <hyperlink ref="B30" r:id="rId29" display="https://www.numbeo.com/cost-of-living/in/Salt-Lake-City" xr:uid="{45DD24BE-5155-8F4E-AB65-4D4360A9E855}"/>
-    <hyperlink ref="B31" r:id="rId30" display="https://www.numbeo.com/cost-of-living/in/Baltimore" xr:uid="{C25F8969-FA84-F141-835D-F64ED8E1409E}"/>
-    <hyperlink ref="B32" r:id="rId31" display="https://www.numbeo.com/cost-of-living/in/Reno" xr:uid="{FF8FB48F-3E5D-0B46-BB63-FF93D5B39D59}"/>
-    <hyperlink ref="B33" r:id="rId32" display="https://www.numbeo.com/cost-of-living/in/New-Orleans" xr:uid="{3F7E73DA-2F06-5A4C-A650-78F3E5E347EA}"/>
-    <hyperlink ref="B34" r:id="rId33" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{4C27741B-9C0B-A346-86E4-DD341E6F95B5}"/>
-    <hyperlink ref="B35" r:id="rId34" display="https://www.numbeo.com/cost-of-living/in/Boise" xr:uid="{FAA7DE53-1FB7-FF4B-B016-D4D6661665CE}"/>
-    <hyperlink ref="B36" r:id="rId35" display="https://www.numbeo.com/cost-of-living/in/Madison" xr:uid="{E033A2A0-01A9-AD46-8967-15CAB34E3EEC}"/>
-    <hyperlink ref="B37" r:id="rId36" display="https://www.numbeo.com/cost-of-living/in/Fort-Worth" xr:uid="{EACD987E-E74A-CE4D-8E2F-E0A0BE340F07}"/>
-    <hyperlink ref="B38" r:id="rId37" display="https://www.numbeo.com/cost-of-living/in/Albuquerque" xr:uid="{97057AD1-B714-CD46-B0C9-12F26B1A937C}"/>
-    <hyperlink ref="B39" r:id="rId38" display="https://www.numbeo.com/cost-of-living/in/Spokane" xr:uid="{FC46AD72-9EB6-D74D-9479-F0409191E3AC}"/>
-    <hyperlink ref="B40" r:id="rId39" display="https://www.numbeo.com/cost-of-living/in/Kansas-City" xr:uid="{85F18226-E87C-EB4C-9B72-14B60AB91274}"/>
-    <hyperlink ref="B41" r:id="rId40" display="https://www.numbeo.com/cost-of-living/in/Greenville" xr:uid="{3EFEBA1C-D39D-8F46-92CD-1BFA7FAACAB8}"/>
-    <hyperlink ref="B42" r:id="rId41" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{FAE5F3CD-D1BA-7A46-9DD5-5DEB6A964513}"/>
-    <hyperlink ref="B43" r:id="rId42" display="https://www.numbeo.com/cost-of-living/in/Las-Vegas" xr:uid="{1FF6BC9A-DD57-0B4C-86CF-390D3DF36F90}"/>
-    <hyperlink ref="B44" r:id="rId43" display="https://www.numbeo.com/cost-of-living/in/Columbus" xr:uid="{E8CB757E-684D-6549-87F8-B8BD3D49462E}"/>
-    <hyperlink ref="B45" r:id="rId44" display="https://www.numbeo.com/cost-of-living/in/Anchorage" xr:uid="{0055400D-6554-BE41-8582-F86E3FF0C932}"/>
-    <hyperlink ref="B46" r:id="rId45" display="https://www.numbeo.com/cost-of-living/in/Jacksonville" xr:uid="{79123DF3-DD60-2742-9737-510F4DCE22D9}"/>
-    <hyperlink ref="B47" r:id="rId46" display="https://www.numbeo.com/cost-of-living/in/Saint-Paul" xr:uid="{76C22C26-5051-814C-86AE-01AB06E3F391}"/>
-    <hyperlink ref="B48" r:id="rId47" display="https://www.numbeo.com/cost-of-living/in/Milwaukee" xr:uid="{A88B1889-1CD4-8F43-A77E-6AA7874DF8EB}"/>
-    <hyperlink ref="B49" r:id="rId48" display="https://www.numbeo.com/cost-of-living/in/Cincinnati" xr:uid="{ACA5E565-F298-E242-8E56-6411D248A268}"/>
-    <hyperlink ref="B50" r:id="rId49" display="https://www.numbeo.com/cost-of-living/in/Richmond" xr:uid="{1E606E0E-0E84-0A43-AAB0-D3035C285CAA}"/>
-    <hyperlink ref="B51" r:id="rId50" display="https://www.numbeo.com/cost-of-living/in/Cleveland" xr:uid="{FDE0CD8C-BA7E-8E44-9A33-7DB33509941A}"/>
-    <hyperlink ref="B52" r:id="rId51" display="https://www.numbeo.com/cost-of-living/in/Buffalo" xr:uid="{9E489D02-C375-0A4D-A6D6-A07AD1E78F4E}"/>
-    <hyperlink ref="B53" r:id="rId52" display="https://www.numbeo.com/cost-of-living/in/Pittsburgh" xr:uid="{14E54EBD-9468-F445-A964-87CF5791C254}"/>
-    <hyperlink ref="B54" r:id="rId53" display="https://www.numbeo.com/cost-of-living/in/Colorado-Springs" xr:uid="{ABB32FD2-7164-F540-BE5E-838C30888E1D}"/>
-    <hyperlink ref="B55" r:id="rId54" display="https://www.numbeo.com/cost-of-living/in/Chattanooga" xr:uid="{36180A5A-8B28-134B-BA67-D832B1EDEEF0}"/>
-    <hyperlink ref="B56" r:id="rId55" display="https://www.numbeo.com/cost-of-living/in/Oklahoma-City" xr:uid="{E03166FE-C34C-904B-A99F-74CE85B00D9F}"/>
-    <hyperlink ref="B57" r:id="rId56" display="https://www.numbeo.com/cost-of-living/in/Birmingham-AL" xr:uid="{46DFF5C4-B8F6-C548-8EAC-5E91179D3E57}"/>
-    <hyperlink ref="B58" r:id="rId57" display="https://www.numbeo.com/cost-of-living/in/Indianapolis" xr:uid="{4A31ABF0-B098-7642-B4ED-8B5450F460BD}"/>
-    <hyperlink ref="B59" r:id="rId58" display="https://www.numbeo.com/cost-of-living/in/Detroit" xr:uid="{48A5FD91-CC29-E245-A53F-841336BC38B9}"/>
-    <hyperlink ref="B60" r:id="rId59" display="https://www.numbeo.com/cost-of-living/in/Tucson" xr:uid="{9B648A9A-8E6E-2D40-830F-768CC422C9BB}"/>
-    <hyperlink ref="B61" r:id="rId60" display="https://www.numbeo.com/cost-of-living/in/Memphis" xr:uid="{B37D6A33-1E46-7E45-B78B-0CA6FFB62C3C}"/>
-    <hyperlink ref="B62" r:id="rId61" display="https://www.numbeo.com/cost-of-living/in/Knoxville" xr:uid="{A67DAB45-1A02-6D43-B0C4-1EB29B2831E3}"/>
-    <hyperlink ref="B63" r:id="rId62" display="https://www.numbeo.com/cost-of-living/in/Saint-Louis" xr:uid="{3195D990-7C89-E54B-BA52-6E35755A0375}"/>
-    <hyperlink ref="B64" r:id="rId63" display="https://www.numbeo.com/cost-of-living/in/Huntsville" xr:uid="{2656E6A0-E821-9148-8752-DF69B89FBE10}"/>
-    <hyperlink ref="B65" r:id="rId64" display="https://www.numbeo.com/cost-of-living/in/Louisville" xr:uid="{5FF0D832-0381-DD4D-A191-B250B4BA3546}"/>
-    <hyperlink ref="B66" r:id="rId65" display="https://www.numbeo.com/cost-of-living/in/Omaha" xr:uid="{874DA96C-52D7-A24E-A249-418AA4BC501E}"/>
-    <hyperlink ref="B67" r:id="rId66" display="https://www.numbeo.com/cost-of-living/in/Tulsa" xr:uid="{391EB714-AE3B-A14D-BCAA-2A31C3F7B269}"/>
+    <hyperlink ref="B10" r:id="rId1" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{505D81DA-7DA7-0E4B-A961-407D8CB180A3}"/>
+    <hyperlink ref="B14" r:id="rId2" display="https://www.numbeo.com/cost-of-living/in/San-Francisco" xr:uid="{3F107AE5-F588-4944-BA28-93A8FE0416B4}"/>
+    <hyperlink ref="B17" r:id="rId3" display="https://www.numbeo.com/cost-of-living/in/Santa-Barbara" xr:uid="{6DCAC14C-23FC-4D43-99A6-13D9E84477BB}"/>
+    <hyperlink ref="B31" r:id="rId4" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{6B5E2C07-E151-2746-8E87-D24F70A057D5}"/>
+    <hyperlink ref="B32" r:id="rId5" display="https://www.numbeo.com/cost-of-living/in/Oakland" xr:uid="{10B6EAF1-FC05-5E4C-A743-0F06A842424D}"/>
+    <hyperlink ref="B38" r:id="rId6" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{658DCA8E-5C0E-224C-B78E-6CAC1EFE822B}"/>
+    <hyperlink ref="B42" r:id="rId7" display="https://www.numbeo.com/cost-of-living/in/San-Jose" xr:uid="{4EE70F74-3CAC-0142-BCBD-48A3717DD8DE}"/>
+    <hyperlink ref="B43" r:id="rId8" display="https://www.numbeo.com/cost-of-living/in/Miami" xr:uid="{96B2F11C-5318-8E40-9210-5DE462401878}"/>
+    <hyperlink ref="B44" r:id="rId9" display="https://www.numbeo.com/cost-of-living/in/Washington" xr:uid="{03E1A461-C305-154B-956F-104282382F8B}"/>
+    <hyperlink ref="B45" r:id="rId10" display="https://www.numbeo.com/cost-of-living/in/Seattle" xr:uid="{6DF47F8F-61E9-CC44-A05F-579FE4701E42}"/>
+    <hyperlink ref="B46" r:id="rId11" display="https://www.numbeo.com/cost-of-living/in/Austin" xr:uid="{D99D0BFA-6C8E-4C40-9D09-B1D990C9FE49}"/>
+    <hyperlink ref="B47" r:id="rId12" display="https://www.numbeo.com/cost-of-living/in/Honolulu" xr:uid="{ABEF44A0-E25D-4C4D-B6DC-1803D593880E}"/>
+    <hyperlink ref="B48" r:id="rId13" display="https://www.numbeo.com/cost-of-living/in/Fort-Lauderdale" xr:uid="{CCFDCB0A-15E2-1F4D-87A9-CA749F786BB4}"/>
+    <hyperlink ref="B49" r:id="rId14" display="https://www.numbeo.com/cost-of-living/in/Tampa" xr:uid="{3D2101C6-1467-A24A-816D-D3E8047DB0DC}"/>
+    <hyperlink ref="B50" r:id="rId15" display="https://www.numbeo.com/cost-of-living/in/Charlotte" xr:uid="{478C7A11-1CA6-994D-9DE8-BD796B6DCC5A}"/>
+    <hyperlink ref="B51" r:id="rId16" display="https://www.numbeo.com/cost-of-living/in/Nashville" xr:uid="{705067BF-7B15-CA41-BA04-463A11DEED40}"/>
+    <hyperlink ref="B57" r:id="rId17" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{CFE3C87A-8C65-8741-9256-67BD8EBBA557}"/>
+    <hyperlink ref="B58" r:id="rId18" display="https://www.numbeo.com/cost-of-living/in/Raleigh" xr:uid="{CD55AD67-D73F-834F-87A8-7F56A6463E1F}"/>
+    <hyperlink ref="B59" r:id="rId19" display="https://www.numbeo.com/cost-of-living/in/Denver" xr:uid="{79516C99-3676-F64F-83C3-A0D706BF5810}"/>
+    <hyperlink ref="B63" r:id="rId20" display="https://www.numbeo.com/cost-of-living/in/Dallas" xr:uid="{D3F59C0C-85A4-5642-B16F-A7E4B0250235}"/>
+    <hyperlink ref="B64" r:id="rId21" display="https://www.numbeo.com/cost-of-living/in/Orlando" xr:uid="{A28F9486-B396-DC4E-8945-DA1E1A7DEEC9}"/>
+    <hyperlink ref="B65" r:id="rId22" display="https://www.numbeo.com/cost-of-living/in/Sacramento" xr:uid="{AF06AE15-18CC-9A4C-A02A-5C2FFC62F127}"/>
+    <hyperlink ref="B66" r:id="rId23" display="https://www.numbeo.com/cost-of-living/in/Portland" xr:uid="{0719E6BF-CB4D-5947-B6F7-A1B3F682B57E}"/>
+    <hyperlink ref="B67" r:id="rId24" display="https://www.numbeo.com/cost-of-living/in/Atlanta" xr:uid="{9BD28DCF-8FA3-3846-8D35-F823EA1E93C0}"/>
+    <hyperlink ref="B77" r:id="rId25" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{FC88C82F-4832-BA44-97A5-A27FBD0F376B}"/>
+    <hyperlink ref="B78" r:id="rId26" display="https://www.numbeo.com/cost-of-living/in/Minneapolis" xr:uid="{C2DC497A-EF35-AF4A-97E3-4060F7E40377}"/>
+    <hyperlink ref="B79" r:id="rId27" display="https://www.numbeo.com/cost-of-living/in/Salt-Lake-City" xr:uid="{45DD24BE-5155-8F4E-AB65-4D4360A9E855}"/>
+    <hyperlink ref="B80" r:id="rId28" display="https://www.numbeo.com/cost-of-living/in/Baltimore" xr:uid="{C25F8969-FA84-F141-835D-F64ED8E1409E}"/>
+    <hyperlink ref="B81" r:id="rId29" display="https://www.numbeo.com/cost-of-living/in/Reno" xr:uid="{FF8FB48F-3E5D-0B46-BB63-FF93D5B39D59}"/>
+    <hyperlink ref="B82" r:id="rId30" display="https://www.numbeo.com/cost-of-living/in/New-Orleans" xr:uid="{3F7E73DA-2F06-5A4C-A650-78F3E5E347EA}"/>
+    <hyperlink ref="B88" r:id="rId31" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{4C27741B-9C0B-A346-86E4-DD341E6F95B5}"/>
+    <hyperlink ref="B89" r:id="rId32" display="https://www.numbeo.com/cost-of-living/in/Boise" xr:uid="{FAA7DE53-1FB7-FF4B-B016-D4D6661665CE}"/>
+    <hyperlink ref="B90" r:id="rId33" display="https://www.numbeo.com/cost-of-living/in/Madison" xr:uid="{E033A2A0-01A9-AD46-8967-15CAB34E3EEC}"/>
+    <hyperlink ref="B91" r:id="rId34" display="https://www.numbeo.com/cost-of-living/in/Fort-Worth" xr:uid="{EACD987E-E74A-CE4D-8E2F-E0A0BE340F07}"/>
+    <hyperlink ref="B92" r:id="rId35" display="https://www.numbeo.com/cost-of-living/in/Albuquerque" xr:uid="{97057AD1-B714-CD46-B0C9-12F26B1A937C}"/>
+    <hyperlink ref="B93" r:id="rId36" display="https://www.numbeo.com/cost-of-living/in/Spokane" xr:uid="{FC46AD72-9EB6-D74D-9479-F0409191E3AC}"/>
+    <hyperlink ref="B94" r:id="rId37" display="https://www.numbeo.com/cost-of-living/in/Kansas-City" xr:uid="{85F18226-E87C-EB4C-9B72-14B60AB91274}"/>
+    <hyperlink ref="B95" r:id="rId38" display="https://www.numbeo.com/cost-of-living/in/Greenville" xr:uid="{3EFEBA1C-D39D-8F46-92CD-1BFA7FAACAB8}"/>
+    <hyperlink ref="B100" r:id="rId39" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{FAE5F3CD-D1BA-7A46-9DD5-5DEB6A964513}"/>
+    <hyperlink ref="B101" r:id="rId40" display="https://www.numbeo.com/cost-of-living/in/Las-Vegas" xr:uid="{1FF6BC9A-DD57-0B4C-86CF-390D3DF36F90}"/>
+    <hyperlink ref="B102" r:id="rId41" display="https://www.numbeo.com/cost-of-living/in/Columbus" xr:uid="{E8CB757E-684D-6549-87F8-B8BD3D49462E}"/>
+    <hyperlink ref="B103" r:id="rId42" display="https://www.numbeo.com/cost-of-living/in/Anchorage" xr:uid="{0055400D-6554-BE41-8582-F86E3FF0C932}"/>
+    <hyperlink ref="B104" r:id="rId43" display="https://www.numbeo.com/cost-of-living/in/Jacksonville" xr:uid="{79123DF3-DD60-2742-9737-510F4DCE22D9}"/>
+    <hyperlink ref="B105" r:id="rId44" display="https://www.numbeo.com/cost-of-living/in/Saint-Paul" xr:uid="{76C22C26-5051-814C-86AE-01AB06E3F391}"/>
+    <hyperlink ref="B106" r:id="rId45" display="https://www.numbeo.com/cost-of-living/in/Milwaukee" xr:uid="{A88B1889-1CD4-8F43-A77E-6AA7874DF8EB}"/>
+    <hyperlink ref="B107" r:id="rId46" display="https://www.numbeo.com/cost-of-living/in/Cincinnati" xr:uid="{ACA5E565-F298-E242-8E56-6411D248A268}"/>
+    <hyperlink ref="B108" r:id="rId47" display="https://www.numbeo.com/cost-of-living/in/Richmond" xr:uid="{1E606E0E-0E84-0A43-AAB0-D3035C285CAA}"/>
+    <hyperlink ref="B109" r:id="rId48" display="https://www.numbeo.com/cost-of-living/in/Cleveland" xr:uid="{FDE0CD8C-BA7E-8E44-9A33-7DB33509941A}"/>
+    <hyperlink ref="B110" r:id="rId49" display="https://www.numbeo.com/cost-of-living/in/Buffalo" xr:uid="{9E489D02-C375-0A4D-A6D6-A07AD1E78F4E}"/>
+    <hyperlink ref="B111" r:id="rId50" display="https://www.numbeo.com/cost-of-living/in/Pittsburgh" xr:uid="{14E54EBD-9468-F445-A964-87CF5791C254}"/>
+    <hyperlink ref="B112" r:id="rId51" display="https://www.numbeo.com/cost-of-living/in/Colorado-Springs" xr:uid="{ABB32FD2-7164-F540-BE5E-838C30888E1D}"/>
+    <hyperlink ref="B113" r:id="rId52" display="https://www.numbeo.com/cost-of-living/in/Chattanooga" xr:uid="{36180A5A-8B28-134B-BA67-D832B1EDEEF0}"/>
+    <hyperlink ref="B114" r:id="rId53" display="https://www.numbeo.com/cost-of-living/in/Oklahoma-City" xr:uid="{E03166FE-C34C-904B-A99F-74CE85B00D9F}"/>
+    <hyperlink ref="B115" r:id="rId54" display="https://www.numbeo.com/cost-of-living/in/Birmingham-AL" xr:uid="{46DFF5C4-B8F6-C548-8EAC-5E91179D3E57}"/>
+    <hyperlink ref="B116" r:id="rId55" display="https://www.numbeo.com/cost-of-living/in/Indianapolis" xr:uid="{4A31ABF0-B098-7642-B4ED-8B5450F460BD}"/>
+    <hyperlink ref="B117" r:id="rId56" display="https://www.numbeo.com/cost-of-living/in/Detroit" xr:uid="{48A5FD91-CC29-E245-A53F-841336BC38B9}"/>
+    <hyperlink ref="B118" r:id="rId57" display="https://www.numbeo.com/cost-of-living/in/Tucson" xr:uid="{9B648A9A-8E6E-2D40-830F-768CC422C9BB}"/>
+    <hyperlink ref="B119" r:id="rId58" display="https://www.numbeo.com/cost-of-living/in/Memphis" xr:uid="{B37D6A33-1E46-7E45-B78B-0CA6FFB62C3C}"/>
+    <hyperlink ref="B120" r:id="rId59" display="https://www.numbeo.com/cost-of-living/in/Knoxville" xr:uid="{A67DAB45-1A02-6D43-B0C4-1EB29B2831E3}"/>
+    <hyperlink ref="B121" r:id="rId60" display="https://www.numbeo.com/cost-of-living/in/Saint-Louis" xr:uid="{3195D990-7C89-E54B-BA52-6E35755A0375}"/>
+    <hyperlink ref="B122" r:id="rId61" display="https://www.numbeo.com/cost-of-living/in/Huntsville" xr:uid="{2656E6A0-E821-9148-8752-DF69B89FBE10}"/>
+    <hyperlink ref="B123" r:id="rId62" display="https://www.numbeo.com/cost-of-living/in/Louisville" xr:uid="{5FF0D832-0381-DD4D-A191-B250B4BA3546}"/>
+    <hyperlink ref="B124" r:id="rId63" display="https://www.numbeo.com/cost-of-living/in/Omaha" xr:uid="{874DA96C-52D7-A24E-A249-418AA4BC501E}"/>
+    <hyperlink ref="B125" r:id="rId64" display="https://www.numbeo.com/cost-of-living/in/Tulsa" xr:uid="{391EB714-AE3B-A14D-BCAA-2A31C3F7B269}"/>
+    <hyperlink ref="B2:B6" r:id="rId65" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{027B5D19-68AD-4049-9572-2D26BBC7BF11}"/>
+    <hyperlink ref="B11:B13" r:id="rId66" display="https://www.numbeo.com/cost-of-living/in/San-Francisco" xr:uid="{01AE3687-C75B-7D42-B521-18212E14C328}"/>
+    <hyperlink ref="B15:B16" r:id="rId67" display="https://www.numbeo.com/cost-of-living/in/San-Francisco" xr:uid="{2A851DC2-DDD0-1240-BE60-09E973DFA3E8}"/>
+    <hyperlink ref="B25" r:id="rId68" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{994B37B3-8D22-7043-A043-80A0D1ADE992}"/>
+    <hyperlink ref="B26" r:id="rId69" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{88E8C901-3DD6-8846-84C8-C5332C4F79DE}"/>
+    <hyperlink ref="B27" r:id="rId70" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{C79D2BAF-93A9-9C41-AF71-75F5B0140CB8}"/>
+    <hyperlink ref="B28" r:id="rId71" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{40581EA5-2DFC-F145-89FD-12171C982E0C}"/>
+    <hyperlink ref="B29" r:id="rId72" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{DD1E1C29-AE77-5E45-B7FC-B72527C9D5F0}"/>
+    <hyperlink ref="B30" r:id="rId73" display="https://www.numbeo.com/cost-of-living/in/Boston" xr:uid="{F7FA8908-9D7E-7142-8FE9-092FB9D9EA51}"/>
+    <hyperlink ref="B7" r:id="rId74" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{55BC3C3A-6DE3-D64B-9D67-B9C5EB7CD8D8}"/>
+    <hyperlink ref="B8" r:id="rId75" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{BC39477B-596E-DA4A-8CE8-BEF704301867}"/>
+    <hyperlink ref="B9" r:id="rId76" display="https://www.numbeo.com/cost-of-living/in/New-York" xr:uid="{45D19051-8789-0047-BBEF-71F0DC9C3AE1}"/>
+    <hyperlink ref="B24" r:id="rId77" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{1FC5B719-FC20-D140-B454-667BEE99C9DC}"/>
+    <hyperlink ref="B18" r:id="rId78" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{B0AB6621-2F70-164E-BCD6-FD6BA027B353}"/>
+    <hyperlink ref="B19" r:id="rId79" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{4F2326AF-9A0B-3B4F-9F9E-046B2AA62455}"/>
+    <hyperlink ref="B20" r:id="rId80" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{4FE7A4A2-8E16-1E4A-BA6B-3D9207AFD1E6}"/>
+    <hyperlink ref="B21" r:id="rId81" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{DC313DCB-43AA-1C41-B83E-D577F991DCD0}"/>
+    <hyperlink ref="B22" r:id="rId82" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{5741E952-2010-4740-9153-E1D74C06A088}"/>
+    <hyperlink ref="B23" r:id="rId83" display="https://www.numbeo.com/cost-of-living/in/San-Diego" xr:uid="{63FF2044-7EB3-7441-B22E-3DFB75807593}"/>
+    <hyperlink ref="B33" r:id="rId84" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{63DF5267-65C9-0146-81D3-E71947A723D7}"/>
+    <hyperlink ref="B34" r:id="rId85" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{FDF72D5B-9011-F048-9824-E284BD37DF39}"/>
+    <hyperlink ref="B35" r:id="rId86" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{D1A65665-9EA6-5847-80AB-7C4560189702}"/>
+    <hyperlink ref="B36" r:id="rId87" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{32DE1203-2444-A944-AE5D-A7809AAFA9D2}"/>
+    <hyperlink ref="B37" r:id="rId88" display="https://www.numbeo.com/cost-of-living/in/Los-Angeles" xr:uid="{1ABA3EA0-B9AE-5B46-9128-4793CB5784D6}"/>
+    <hyperlink ref="B52" r:id="rId89" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{0C7F817E-56D9-A546-8D17-BE012D0DAA50}"/>
+    <hyperlink ref="B53" r:id="rId90" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{F35121BE-8DF3-DA47-B649-B0AE6E8EE341}"/>
+    <hyperlink ref="B54" r:id="rId91" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{1C923090-C97E-D640-982C-27040CA35D77}"/>
+    <hyperlink ref="B55" r:id="rId92" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{A2560D78-4982-534D-9EA4-1FD1F8340B77}"/>
+    <hyperlink ref="B56" r:id="rId93" display="https://www.numbeo.com/cost-of-living/in/Chicago" xr:uid="{E39A3C3F-9F2C-4146-B0C6-40C1E4E1B075}"/>
+    <hyperlink ref="B83" r:id="rId94" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{73C5D097-A4D4-6C43-AF47-5DE6A7150F75}"/>
+    <hyperlink ref="B84" r:id="rId95" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{A228A847-8BA5-7942-890A-B5D2DC5A6387}"/>
+    <hyperlink ref="B85" r:id="rId96" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{37486724-9155-4447-8C34-070439F0F9A6}"/>
+    <hyperlink ref="B86" r:id="rId97" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{FDAF56C9-9F89-1A41-B9FA-F7D521315167}"/>
+    <hyperlink ref="B87" r:id="rId98" display="https://www.numbeo.com/cost-of-living/in/Houston" xr:uid="{A69BFD3E-759E-CF48-B1B2-5221C31E9B9A}"/>
+    <hyperlink ref="B68" r:id="rId99" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{A2A89FD1-4A7A-9846-B5D1-64FEFEA5D583}"/>
+    <hyperlink ref="B70" r:id="rId100" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{70318A2F-CBDA-DD4B-82BC-585D6BB78D1C}"/>
+    <hyperlink ref="B71" r:id="rId101" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{C0182929-1BF0-9248-86A5-5289B5672270}"/>
+    <hyperlink ref="B72" r:id="rId102" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{386A3157-B4DD-2B41-B58B-7E92EFD7EF19}"/>
+    <hyperlink ref="B69" r:id="rId103" display="https://www.numbeo.com/cost-of-living/in/Phoenix" xr:uid="{E6CD9788-7F97-434E-997C-2AC0A471E0E8}"/>
+    <hyperlink ref="B73" r:id="rId104" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{B41CE8D4-6B78-654C-AA8C-662F99F2A85C}"/>
+    <hyperlink ref="B74" r:id="rId105" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{194AD1AB-14DF-3248-BA39-8AD0761EE8A4}"/>
+    <hyperlink ref="B75" r:id="rId106" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{19903E92-C072-C946-A3B1-7699E5645BB8}"/>
+    <hyperlink ref="B76" r:id="rId107" display="https://www.numbeo.com/cost-of-living/in/Philadelphia" xr:uid="{E4EB080F-AA1E-2843-B36D-0E64F340CFB5}"/>
+    <hyperlink ref="B96" r:id="rId108" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{16F30AF9-BE8B-7B48-BF19-0DDD54C3B556}"/>
+    <hyperlink ref="B97" r:id="rId109" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{D2CBECCB-4667-4A48-8C26-D353F683EA6E}"/>
+    <hyperlink ref="B98" r:id="rId110" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{8A3CE4D6-0829-3F45-BBA1-E971593D7BB8}"/>
+    <hyperlink ref="B99" r:id="rId111" display="https://www.numbeo.com/cost-of-living/in/San-Antonio" xr:uid="{D5181D38-4C94-3F47-90A6-03D2ECE727FA}"/>
+    <hyperlink ref="B60" r:id="rId112" display="https://www.numbeo.com/cost-of-living/in/Dallas" xr:uid="{81B000F4-45E1-6A4A-B636-4BB7CC9BC6F1}"/>
+    <hyperlink ref="B61" r:id="rId113" display="https://www.numbeo.com/cost-of-living/in/Dallas" xr:uid="{631C43B1-A8EF-3148-A817-5720846DD62B}"/>
+    <hyperlink ref="B62" r:id="rId114" display="https://www.numbeo.com/cost-of-living/in/Dallas" xr:uid="{854DC0E1-6D41-FF4A-944E-ECEC4BB98DB2}"/>
+    <hyperlink ref="B39" r:id="rId115" display="https://www.numbeo.com/cost-of-living/in/San-Jose" xr:uid="{5F27411B-71E6-A847-9D5F-CE82153AF2E0}"/>
+    <hyperlink ref="B40" r:id="rId116" display="https://www.numbeo.com/cost-of-living/in/San-Jose" xr:uid="{F4E6A442-2B3B-4D43-AD10-4A3324559D38}"/>
+    <hyperlink ref="B41" r:id="rId117" display="https://www.numbeo.com/cost-of-living/in/San-Jose" xr:uid="{63FBC2E5-C318-0440-8ED2-47F377ECF752}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>